<commit_message>
Started refactoring to allow for model loading, texturing, instancing, and N-Model Updating/Rendering
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="79">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -365,6 +365,9 @@
   </si>
   <si>
     <t>Student Git Address: https://github.com/exlted/Graphics-2-Project.git</t>
+  </si>
+  <si>
+    <t>http://www.opengl-tutorial.org/beginners-tutorials/tutorial-7-model-loading/</t>
   </si>
 </sst>
 </file>
@@ -929,7 +932,7 @@
   <dimension ref="A1:L117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2945,7 +2948,9 @@
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A95" s="13"/>
+      <c r="A95" s="13" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="13"/>

</xml_diff>

<commit_message>
Added new shaders, graphical systems, etc. Cube is working Problems with loaded model, all faces being culled before pixel shader runs
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="81">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -368,6 +368,12 @@
   </si>
   <si>
     <t>http://www.opengl-tutorial.org/beginners-tutorials/tutorial-7-model-loading/</t>
+  </si>
+  <si>
+    <t>http://www.3dgep.com/texturing-lighting-directx-11/#Multiple_Instance_Vertex_Shader</t>
+  </si>
+  <si>
+    <t>I</t>
   </si>
 </sst>
 </file>
@@ -932,7 +938,7 @@
   <dimension ref="A1:L117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1048,7 +1054,9 @@
       <c r="D4" s="5">
         <v>2</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="F4" s="3"/>
       <c r="G4" s="17">
         <f t="shared" ref="G4:G35" si="0" xml:space="preserve"> IF(EXACT(F4,"X"),IF(EXACT(E4,"I"),$B4,IF(EXACT(E4,"II"),$C4,IF(EXACT(E4,"III"),$D4,0))),0)</f>
@@ -2426,7 +2434,9 @@
       <c r="D65" s="5">
         <v>1</v>
       </c>
-      <c r="E65" s="2"/>
+      <c r="E65" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="F65" s="3"/>
       <c r="G65" s="17">
         <f t="shared" si="1"/>
@@ -2451,7 +2461,9 @@
       <c r="D66" s="5">
         <v>1</v>
       </c>
-      <c r="E66" s="2"/>
+      <c r="E66" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="F66" s="3"/>
       <c r="G66" s="17">
         <f t="shared" si="1"/>
@@ -2953,7 +2965,9 @@
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A96" s="13"/>
+      <c r="A96" s="13" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="13"/>
@@ -3040,7 +3054,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Refactored Cube to work in my RenderSystem, Finished getting ModelLoading to work, some issues still with texturing
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="81">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -937,24 +937,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="101.25" customWidth="1"/>
-    <col min="2" max="2" width="25.375" customWidth="1"/>
+    <col min="1" max="1" width="101.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="25.25" customWidth="1"/>
-    <col min="5" max="5" width="25.625" customWidth="1"/>
-    <col min="6" max="6" width="25.375" customWidth="1"/>
-    <col min="7" max="7" width="25.75" customWidth="1"/>
-    <col min="8" max="9" width="25.875" customWidth="1"/>
-    <col min="10" max="10" width="24.75" customWidth="1"/>
-    <col min="11" max="11" width="24.625" customWidth="1"/>
-    <col min="12" max="12" width="24.125" customWidth="1"/>
-    <col min="13" max="14" width="9.125" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="8" max="9" width="25.85546875" customWidth="1"/>
+    <col min="10" max="10" width="24.7109375" customWidth="1"/>
+    <col min="11" max="11" width="24.5703125" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" customWidth="1"/>
+    <col min="13" max="14" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -1096,7 +1096,9 @@
       <c r="D5" s="5">
         <v>2</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="F5" s="3"/>
       <c r="G5" s="17">
         <f t="shared" si="0"/>
@@ -3054,7 +3056,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Should now work without any extra work post-compilation Started work on Instancing Models
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -938,7 +938,7 @@
   <dimension ref="A1:L117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3060,7 +3060,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Started a bit of work on specular mapping Finished quick material library Changed modelLoading to import specular as well Possible missed minor changes
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="81">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -937,8 +937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1431,7 +1431,9 @@
       <c r="D18" s="5">
         <v>2</v>
       </c>
-      <c r="E18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="F18" s="3"/>
       <c r="G18" s="17">
         <f t="shared" si="0"/>
@@ -1955,7 +1957,9 @@
       <c r="D40" s="5">
         <v>2</v>
       </c>
-      <c r="E40" s="2"/>
+      <c r="E40" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="F40" s="3"/>
       <c r="G40" s="17">
         <f t="shared" si="1"/>
@@ -3072,7 +3076,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Normal Mapping now works (Currently flips normal mapping on and off every 5 seconds on the Turret)
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="81">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -937,8 +937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1508,7 +1508,9 @@
       <c r="D21" s="5">
         <v>2</v>
       </c>
-      <c r="E21" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="F21" s="3"/>
       <c r="G21" s="17">
         <f t="shared" si="0"/>
@@ -1533,7 +1535,9 @@
       <c r="D22" s="5">
         <v>2</v>
       </c>
-      <c r="E22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="F22" s="3"/>
       <c r="G22" s="17">
         <f t="shared" si="0"/>
@@ -1907,7 +1911,9 @@
       <c r="D38" s="5">
         <v>2</v>
       </c>
-      <c r="E38" s="2"/>
+      <c r="E38" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="F38" s="3"/>
       <c r="G38" s="17">
         <f t="shared" si="1"/>
@@ -1932,7 +1938,9 @@
       <c r="D39" s="5">
         <v>2</v>
       </c>
-      <c r="E39" s="2"/>
+      <c r="E39" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="F39" s="3"/>
       <c r="G39" s="17">
         <f t="shared" si="1"/>
@@ -3076,7 +3084,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Skybox known non-working, must fix later
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="82">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -374,6 +374,9 @@
   </si>
   <si>
     <t>I</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -937,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1057,14 +1060,16 @@
       <c r="E4" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="G4" s="17">
         <f t="shared" ref="G4:G35" si="0" xml:space="preserve"> IF(EXACT(F4,"X"),IF(EXACT(E4,"I"),$B4,IF(EXACT(E4,"II"),$C4,IF(EXACT(E4,"III"),$D4,0))),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H4" s="18">
         <f>IF(SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91) &gt; 18, 18, SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91))</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="I4" s="18">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 18, 18, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91))</f>
@@ -1076,11 +1081,11 @@
       </c>
       <c r="K4" s="18">
         <f>SUM(H6,I6,J6)</f>
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="L4" s="18">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>0</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1099,10 +1104,12 @@
       <c r="E5" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="G5" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>27</v>
@@ -1134,14 +1141,16 @@
       <c r="E6" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="G6" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H6" s="18">
         <f>IF(SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91)  &gt; 18, SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91) - 18,0)</f>
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="I6" s="18">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 18, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) - 18,0)</f>
@@ -1209,15 +1218,15 @@
       </c>
       <c r="H8" s="19">
         <f>H4+IF(H4 &lt; 18, IF(K4+H4 &gt; 18, 18- H4, K4),0)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="I8" s="18">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="J8" s="18">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1274,11 +1283,11 @@
       </c>
       <c r="H10" s="20">
         <f>IF(K4+H4 - 18 &gt; 0, K4+H4 - 18, 0)</f>
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="I10" s="20">
         <f>IF(H10+I4 - 18 &gt; 0, H10+I4 - 18, 0)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J10" s="20">
         <f>IF(I10+J4 - 18 &gt; 0, I10+J4 - 18, 0)</f>
@@ -1434,10 +1443,12 @@
       <c r="E18" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F18" s="3"/>
+      <c r="F18" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="G18" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
@@ -1511,10 +1522,12 @@
       <c r="E21" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F21" s="3"/>
+      <c r="F21" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="G21" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -1538,10 +1551,12 @@
       <c r="E22" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F22" s="3"/>
+      <c r="F22" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="G22" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
@@ -1562,9 +1577,7 @@
       <c r="D23" s="5">
         <v>3</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>80</v>
-      </c>
+      <c r="E23" s="2"/>
       <c r="F23" s="3"/>
       <c r="G23" s="17">
         <f t="shared" si="0"/>
@@ -1704,10 +1717,12 @@
       <c r="E30" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F30" s="3"/>
+      <c r="F30" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="G30" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
@@ -1731,10 +1746,12 @@
       <c r="E31" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F31" s="3"/>
+      <c r="F31" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="G31" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -1758,10 +1775,12 @@
       <c r="E32" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F32" s="3"/>
+      <c r="F32" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="G32" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
@@ -1785,10 +1804,12 @@
       <c r="E33" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F33" s="3"/>
+      <c r="F33" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="G33" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
@@ -1809,11 +1830,15 @@
       <c r="D34" s="5">
         <v>1</v>
       </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="3"/>
+      <c r="E34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="G34" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
@@ -1837,10 +1862,12 @@
       <c r="E35" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F35" s="3"/>
+      <c r="F35" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="G35" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
@@ -1861,11 +1888,15 @@
       <c r="D36" s="5">
         <v>1</v>
       </c>
-      <c r="E36" s="2"/>
-      <c r="F36" s="3"/>
+      <c r="E36" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="G36" s="17">
         <f t="shared" ref="G36:G67" si="1" xml:space="preserve"> IF(EXACT(F36,"X"),IF(EXACT(E36,"I"),$B36,IF(EXACT(E36,"II"),$C36,IF(EXACT(E36,"III"),$D36,0))),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
@@ -1914,10 +1945,12 @@
       <c r="E38" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F38" s="3"/>
+      <c r="F38" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="G38" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
@@ -1941,10 +1974,12 @@
       <c r="E39" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F39" s="3"/>
+      <c r="F39" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="G39" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
@@ -1968,10 +2003,12 @@
       <c r="E40" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F40" s="3"/>
+      <c r="F40" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="G40" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
@@ -2269,10 +2306,12 @@
       <c r="E55" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F55" s="3"/>
+      <c r="F55" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="G55" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
@@ -2467,10 +2506,12 @@
       <c r="E65" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F65" s="3"/>
+      <c r="F65" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="G65" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
@@ -2494,10 +2535,12 @@
       <c r="E66" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F66" s="3"/>
+      <c r="F66" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="G66" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
@@ -2927,7 +2970,9 @@
       <c r="B90" s="6">
         <v>2</v>
       </c>
-      <c r="C90" s="3"/>
+      <c r="C90" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
       <c r="F90" s="5"/>
@@ -2945,7 +2990,9 @@
       <c r="B91" s="6">
         <v>1</v>
       </c>
-      <c r="C91" s="3"/>
+      <c r="C91" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
       <c r="F91" s="5"/>
@@ -3084,7 +3131,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Started working on post processing
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -940,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3131,7 +3131,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Finished rendering Render to Texture texture on Turret in scene, turned off grayscale post processing to make texture more apparent
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -79,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="84">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -380,6 +381,9 @@
   </si>
   <si>
     <t>II</t>
+  </si>
+  <si>
+    <t>III</t>
   </si>
 </sst>
 </file>
@@ -977,8 +981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D90" sqref="D90"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,7 +1118,7 @@
       </c>
       <c r="J4" s="18">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 18, 18, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K4" s="18">
         <f>SUM(H6,I6,J6)</f>
@@ -1122,7 +1126,7 @@
       </c>
       <c r="L4" s="18">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1200,7 +1204,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="16">
         <f>IF(L4 &gt; 54, SUM(-54,L4),0)</f>
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1328,7 +1332,7 @@
       </c>
       <c r="J10" s="20">
         <f>IF(I10+J4 - 18 &gt; 0, I10+J4 - 18, 0)</f>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -1531,11 +1535,15 @@
       <c r="D20" s="5">
         <v>4</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="3"/>
+      <c r="E20" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="G20" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -3017,7 +3025,9 @@
       <c r="D90" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E90" s="3"/>
+      <c r="E90" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="F90" s="5"/>
       <c r="G90" s="5"/>
       <c r="H90" s="5"/>
@@ -3039,7 +3049,9 @@
       <c r="D91" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E91" s="3"/>
+      <c r="E91" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
       <c r="H91" s="5"/>

</xml_diff>